<commit_message>
Seed database with all priority levels
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livesmucac-my.sharepoint.com/personal/2416130_live_stmarys_ac_uk/Documents/Software Engineering/Final Assessment/emergency-resource-allocation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C66B80F1-DBF4-4CF7-972E-D3C8FA12FBC7}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23ECD367-136C-4FEF-A410-8EBC0E36BFDC}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="16440" windowHeight="28320" firstSheet="4" activeTab="6" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="4" activeTab="4" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
     <sheet name="emergency" sheetId="2" r:id="rId2"/>
     <sheet name="emergency_type" sheetId="5" r:id="rId3"/>
     <sheet name="emergency_type_severity_resourc" sheetId="6" r:id="rId4"/>
-    <sheet name="priority_level" sheetId="3" r:id="rId5"/>
+    <sheet name="priority" sheetId="3" r:id="rId5"/>
     <sheet name="resources" sheetId="4" r:id="rId6"/>
     <sheet name="resource_type" sheetId="7" r:id="rId7"/>
     <sheet name="incident_resource" sheetId="8" r:id="rId8"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>zone</t>
   </si>
@@ -66,12 +66,6 @@
     <t>emergency</t>
   </si>
   <si>
-    <t>priority_level_id</t>
-  </si>
-  <si>
-    <t>priority_level</t>
-  </si>
-  <si>
     <t>Low risk</t>
   </si>
   <si>
@@ -160,6 +154,9 @@
   </si>
   <si>
     <t>resource_type_id</t>
+  </si>
+  <si>
+    <t>priority_id</t>
   </si>
 </sst>
 </file>
@@ -215,6 +212,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -621,10 +622,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -632,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -640,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -648,7 +649,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -656,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -664,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -672,7 +673,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -680,7 +681,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -704,19 +705,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -760,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDD8D38-8054-498C-8E82-67EBB6B2667F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -773,10 +774,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -790,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -801,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -812,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -836,10 +837,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -883,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580C13D8-4112-42D0-92D0-4E33466078A9}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -896,10 +897,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -910,10 +911,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -921,10 +922,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -932,10 +933,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -943,10 +944,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -969,10 +970,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Seed the database with locations
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livesmucac-my.sharepoint.com/personal/2416130_live_stmarys_ac_uk/Documents/Software Engineering/Final Assessment/emergency-resource-allocation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23ECD367-136C-4FEF-A410-8EBC0E36BFDC}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E5B711F-85A6-4F1D-8D59-E0014F485C90}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="4" activeTab="4" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>zone</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>priority_id</t>
+  </si>
+  <si>
+    <t>x_coordinate</t>
+  </si>
+  <si>
+    <t>y_coordinate</t>
+  </si>
+  <si>
+    <t>location_id</t>
   </si>
 </sst>
 </file>
@@ -535,47 +544,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8FC51C-8777-4C3C-A2F1-B54D301975FE}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDD8D38-8054-498C-8E82-67EBB6B2667F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Seed emergency type priority resource
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livesmucac-my.sharepoint.com/personal/2416130_live_stmarys_ac_uk/Documents/Software Engineering/Final Assessment/emergency-resource-allocation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E5B711F-85A6-4F1D-8D59-E0014F485C90}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CEE98EC-08B3-413F-9C3C-3E99CFB71D38}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="3" activeTab="5" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
     <sheet name="emergency" sheetId="2" r:id="rId2"/>
     <sheet name="emergency_type" sheetId="5" r:id="rId3"/>
-    <sheet name="emergency_type_severity_resourc" sheetId="6" r:id="rId4"/>
+    <sheet name="emergency_type_priority_resourc" sheetId="6" r:id="rId4"/>
     <sheet name="priority" sheetId="3" r:id="rId5"/>
-    <sheet name="resources" sheetId="4" r:id="rId6"/>
+    <sheet name="resource" sheetId="4" r:id="rId6"/>
     <sheet name="resource_type" sheetId="7" r:id="rId7"/>
     <sheet name="incident_resource" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>zone</t>
   </si>
@@ -102,21 +102,6 @@
     <t>Sexual Assault</t>
   </si>
   <si>
-    <t>emergency_type_severity_resource_id</t>
-  </si>
-  <si>
-    <t>emergency_type</t>
-  </si>
-  <si>
-    <t>severity</t>
-  </si>
-  <si>
-    <t>resource</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
     <t>resource_id</t>
   </si>
   <si>
@@ -166,6 +151,12 @@
   </si>
   <si>
     <t>location_id</t>
+  </si>
+  <si>
+    <t>emergency_type_priority_resource_id</t>
+  </si>
+  <si>
+    <t>recommended_quantity</t>
   </si>
 </sst>
 </file>
@@ -201,11 +192,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8FC51C-8777-4C3C-A2F1-B54D301975FE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -558,16 +550,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -728,30 +720,33 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="30.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.46484375" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -761,12 +756,30 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
     </row>
@@ -777,6 +790,15 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
@@ -784,6 +806,15 @@
       </c>
       <c r="B5">
         <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -808,7 +839,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -857,10 +888,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E901C1EC-7FD9-4045-AE98-D7AD68A18F79}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -871,17 +902,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
     </row>
@@ -889,7 +920,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -897,7 +928,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -905,8 +936,200 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2.3571428571428501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.5476190476190399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.7380952380952301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2.9285714285714199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3.11904761904762</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3.3095238095238102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3.6904761904761898</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3.88095238095238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4.0714285714285703</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4.2619047619047601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4.4523809523809499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2.3571428571428501</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -945,10 +1168,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -956,10 +1179,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -967,10 +1190,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -978,10 +1201,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1004,10 +1227,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Seed all database tables
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livesmucac-my.sharepoint.com/personal/2416130_live_stmarys_ac_uk/Documents/Software Engineering/Final Assessment/emergency-resource-allocation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CEE98EC-08B3-413F-9C3C-3E99CFB71D38}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B013DC7A-A9C9-4971-A46F-445DC70DAC41}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="3" activeTab="5" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="9" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
-    <sheet name="emergency" sheetId="2" r:id="rId2"/>
-    <sheet name="emergency_type" sheetId="5" r:id="rId3"/>
-    <sheet name="emergency_type_priority_resourc" sheetId="6" r:id="rId4"/>
-    <sheet name="priority" sheetId="3" r:id="rId5"/>
-    <sheet name="resource" sheetId="4" r:id="rId6"/>
-    <sheet name="resource_type" sheetId="7" r:id="rId7"/>
-    <sheet name="incident_resource" sheetId="8" r:id="rId8"/>
+    <sheet name="incident" sheetId="10" r:id="rId2"/>
+    <sheet name="emergency" sheetId="2" r:id="rId3"/>
+    <sheet name="emergency_type" sheetId="5" r:id="rId4"/>
+    <sheet name="emergency_type_priority_resourc" sheetId="6" r:id="rId5"/>
+    <sheet name="priority" sheetId="3" r:id="rId6"/>
+    <sheet name="resource" sheetId="4" r:id="rId7"/>
+    <sheet name="incident_emergency_type_priorit" sheetId="9" r:id="rId8"/>
+    <sheet name="resource_type" sheetId="7" r:id="rId9"/>
+    <sheet name="incident_resource" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>zone</t>
   </si>
@@ -157,6 +159,33 @@
   </si>
   <si>
     <t>recommended_quantity</t>
+  </si>
+  <si>
+    <t>incident_id</t>
+  </si>
+  <si>
+    <t>incident_emergency_type_priority_resource_id</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Fire a wharehouse</t>
+  </si>
+  <si>
+    <t>Mass shooting &amp; stabbing</t>
+  </si>
+  <si>
+    <t>Flooding</t>
+  </si>
+  <si>
+    <t>Chemical spill</t>
+  </si>
+  <si>
+    <t>Heart attack</t>
+  </si>
+  <si>
+    <t>resource</t>
   </si>
 </sst>
 </file>
@@ -609,7 +638,155 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB6154-8A15-43C3-870C-290585DC8636}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C945EA-EA60-4562-9A52-ADDE24A4A581}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="20.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECDFF43-02A1-4E93-A1CF-077A42E19C88}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -632,7 +809,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF54C46-220D-4E57-B4A6-7502E747BB32}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -715,7 +892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F12F16-10C9-43F9-A82C-C795B50B5417}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -822,7 +999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDD8D38-8054-498C-8E82-67EBB6B2667F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -886,11 +1063,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E901C1EC-7FD9-4045-AE98-D7AD68A18F79}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24:A29"/>
     </sheetView>
   </sheetViews>
@@ -1137,7 +1314,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C9C51E-5D7D-436B-8BF4-6611AB23AC99}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580C13D8-4112-42D0-92D0-4E33466078A9}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1210,54 +1429,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB6154-8A15-43C3-870C-290585DC8636}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="18.19921875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Create front-end menu for user interface
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livesmucac-my.sharepoint.com/personal/2416130_live_stmarys_ac_uk/Documents/Software Engineering/Final Assessment/emergency-resource-allocation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B013DC7A-A9C9-4971-A46F-445DC70DAC41}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="8_{C401EFCD-EF72-443A-A931-E8B161BD40E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C53BAEE-21A3-4B82-B0F6-4C9B4CD25870}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="9" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="6" activeTab="10" xr2:uid="{290CB0C5-5BD9-42C4-9590-F0B0A9F82338}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="incident_emergency_type_priorit" sheetId="9" r:id="rId8"/>
     <sheet name="resource_type" sheetId="7" r:id="rId9"/>
     <sheet name="incident_resource" sheetId="8" r:id="rId10"/>
+    <sheet name="status" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>zone</t>
   </si>
@@ -186,6 +187,30 @@
   </si>
   <si>
     <t>resource</t>
+  </si>
+  <si>
+    <t>status_id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
+    <t>Unsure</t>
+  </si>
+  <si>
+    <t>Incident resolved</t>
+  </si>
+  <si>
+    <t>Incident ongoing</t>
+  </si>
+  <si>
+    <t>Unclear as to resolution/continuation of incident</t>
   </si>
 </sst>
 </file>
@@ -642,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB6154-8A15-43C3-870C-290585DC8636}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -702,21 +727,85 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C945EA-EA60-4562-9A52-ADDE24A4A581}">
-  <dimension ref="A1:C6"/>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8858CA-D1A6-473B-BAEE-E365B6E64604}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C945EA-EA60-4562-9A52-ADDE24A4A581}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
         <v>38</v>
       </c>
       <c r="B1" t="s">
@@ -725,8 +814,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -736,8 +828,11 @@
       <c r="C2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -747,8 +842,11 @@
       <c r="C3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -758,8 +856,11 @@
       <c r="C4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -769,8 +870,11 @@
       <c r="C5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -779,6 +883,9 @@
       </c>
       <c r="C6" t="s">
         <v>45</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>